<commit_message>
fixed date format of uploading parts
</commit_message>
<xml_diff>
--- a/api-server/public/bacterium_template.xlsx
+++ b/api-server/public/bacterium_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10988"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,18 +69,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -504,27 +504,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.53125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.53125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.73046875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.19921875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.53125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.19921875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.46484375" customWidth="1"/>
-    <col min="11" max="11" width="18.9296875" customWidth="1"/>
-    <col min="12" max="12" width="23.46484375" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.453125" customWidth="1"/>
+    <col min="11" max="11" width="18.90625" customWidth="1"/>
+    <col min="12" max="12" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="49.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="49.9" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>